<commit_message>
Register page + favicon + profile page started
</commit_message>
<xml_diff>
--- a/munkanaplo.xlsx
+++ b/munkanaplo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\root\google-drives\mindszenti.gergo\studies\university\subjects\23-24_2\webtervezes\gy\projektmunka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\root\google-drives\pr01.storage.mg\programming\web-projects\hirdeto-kereskedelmi-oldal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3746B1A2-C0F5-436B-AC2B-95E050EA9D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1C7D90-6FA3-4AEB-B5A5-322613EDCC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{887FEA99-DCDB-4888-A6E5-5E03AEB02C52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Időpont</t>
   </si>
@@ -51,6 +51,54 @@
   </si>
   <si>
     <t>Problémák / nehézségek / megoldások</t>
+  </si>
+  <si>
+    <t>március 8</t>
+  </si>
+  <si>
+    <t>mindenki</t>
+  </si>
+  <si>
+    <t>február 14</t>
+  </si>
+  <si>
+    <t>csapat kialakítása</t>
+  </si>
+  <si>
+    <t>megbeszéltük, hogy mindkettőnknek ötös a célja, így jól fog menni a csapatmunka</t>
+  </si>
+  <si>
+    <t>február 18</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>csapatnév kitalálása és regisztrálása</t>
+  </si>
+  <si>
+    <t>március 5</t>
+  </si>
+  <si>
+    <t>projekttéma kiválasztása</t>
+  </si>
+  <si>
+    <t>projekt tématerv megírása és beküldése</t>
+  </si>
+  <si>
+    <t>összeültünk egy órára, és közösen megbeszéltük az alapvető funkciókat, oldalakat</t>
+  </si>
+  <si>
+    <t>március 19</t>
+  </si>
+  <si>
+    <t>Mindszenti Gergő</t>
+  </si>
+  <si>
+    <t>GitHub repo létrehozása</t>
+  </si>
+  <si>
+    <t>regisztrációs/bejelentkező oldal megalkotása</t>
   </si>
 </sst>
 </file>
@@ -563,7 +611,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,27 +646,85 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>